<commit_message>
Update figs 01, 02, 04, 06, 08
</commit_message>
<xml_diff>
--- a/vaw/data/list_of_tables_for_summary.xlsx
+++ b/vaw/data/list_of_tables_for_summary.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="75" windowWidth="20115" windowHeight="7995"/>
+    <workbookView xWindow="240" yWindow="75" windowWidth="20115" windowHeight="7845"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="89">
   <si>
     <t>Figures</t>
   </si>
@@ -308,12 +308,319 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
+      <t xml:space="preserve">Figure 34. </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Differences among women aged 65+ in EU countries for self-rated health very good-good by wealth quintiles, 2013</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Figure 37. </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Long-term pyschological consequences of violence as a result of physical and sexual violence by a partner reported by women 60+ years in the EU</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Figure 38. </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Differences among older women by age in poverty risk for 2013</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Figure 5. </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Global Gender Gap for 47 Member States of the WHO European Region 2014</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Figure 27c. </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Unmet needs for family planning, total, percentage (last year available) </t>
+    </r>
+  </si>
+  <si>
+    <t>countries</t>
+  </si>
+  <si>
+    <t>number of years</t>
+  </si>
+  <si>
+    <t>Beyond the mortality advantage</t>
+  </si>
+  <si>
+    <t>as in doc</t>
+  </si>
+  <si>
+    <t>Note</t>
+  </si>
+  <si>
+    <t>sub regions</t>
+  </si>
+  <si>
+    <t>deaths and DALYs</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Score </t>
+  </si>
+  <si>
+    <t>percentage</t>
+  </si>
+  <si>
+    <t>Are we maximazing the education gain?</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Figure 16a. The </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Risk of poverty and social exclusion for girls age less than 6 years in the EU, 2013</t>
+    </r>
+  </si>
+  <si>
+    <t>prevalence</t>
+  </si>
+  <si>
+    <t>number of responses</t>
+  </si>
+  <si>
+    <t>Notes:</t>
+  </si>
+  <si>
+    <t>X and Y lables are as they should be in the graphs as per current draft. However, you will probably change them if presenting the data in a different form, as with the example you shown as on violence Fig 37.</t>
+  </si>
+  <si>
+    <t>Number and name of figure as per draft document</t>
+  </si>
+  <si>
+    <t>Proposed subtitle</t>
+  </si>
+  <si>
+    <t>Page no (in draft doc)</t>
+  </si>
+  <si>
+    <t>Reference no (as per in draft doc)</t>
+  </si>
+  <si>
+    <t>Girls opportunities for early development</t>
+  </si>
+  <si>
+    <t>Unequal pay for women in all countries</t>
+  </si>
+  <si>
+    <t>Source</t>
+  </si>
+  <si>
+    <t>Link</t>
+  </si>
+  <si>
+    <t>Data accessed</t>
+  </si>
+  <si>
+    <t>WHO. Life expectancy. Data by country [web site].</t>
+  </si>
+  <si>
+    <t>http://apps.who.int/gho/data/node.main.3?lang=en</t>
+  </si>
+  <si>
+    <t>United Nations Development Programme (UNDP)</t>
+  </si>
+  <si>
+    <t>http://hdr.undp.org/en/content/table-4-gender-inequality-index</t>
+  </si>
+  <si>
+    <t>IHME 2010</t>
+  </si>
+  <si>
+    <t>http://vizhub.healthdata.org/irank/arrow.php</t>
+  </si>
+  <si>
+    <t>Accessed 16 March 2015</t>
+  </si>
+  <si>
+    <t>Accessed 28 March 2015</t>
+  </si>
+  <si>
+    <t>World Economic Forum (WEF)</t>
+  </si>
+  <si>
+    <t>http://reports.weforum.org/global-gender-gap-report-2014/rankings/</t>
+  </si>
+  <si>
+    <t>Eurostat</t>
+  </si>
+  <si>
+    <t>http://ec.europa.eu/eurostat/tgm/table.do?tab=table&amp;init=1&amp;plugin=1&amp;language=en&amp;pcode=tsdsc340</t>
+  </si>
+  <si>
+    <t>European Health for All Database (HFA, DB), WHO/Europe</t>
+  </si>
+  <si>
+    <t>Accessed 22 April 2015</t>
+  </si>
+  <si>
+    <t>http://data.euro.who.int/hfadb/</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Unicef 2015 State of the World’s Children </t>
+  </si>
+  <si>
+    <t>http://www.data.unicef.org/resources/the-state-of-the-world-s-children-report-2015-statistical-tables</t>
+  </si>
+  <si>
+    <t>Accessed on 26 April 2015</t>
+  </si>
+  <si>
+    <t>http://ec.europa.eu/eurostat/web/products-datasets/-/t2020_50</t>
+  </si>
+  <si>
+    <t>Accessed 16 June 2015</t>
+  </si>
+  <si>
+    <t>http://nccd.cdc.gov/gtssdata/Ancillary/Documentation.aspx?SUID=1&amp;DOCT=1</t>
+  </si>
+  <si>
+    <t>Global Youth Tobacco Survey (GYTS)</t>
+  </si>
+  <si>
+    <t>Accessed 10 July 2015</t>
+  </si>
+  <si>
+    <t>Accessed 30 June 2015</t>
+  </si>
+  <si>
+    <t>Accessed 23 June 2015</t>
+  </si>
+  <si>
+    <t>Accessed 13 July 2015</t>
+  </si>
+  <si>
+    <t>Accessed 31 May 2015</t>
+  </si>
+  <si>
+    <t xml:space="preserve">http://www.unicef.org/sowc2011/fullreport.php </t>
+  </si>
+  <si>
+    <t>Wrong reference in the Draft Report to 2011 Unicef report instead of the 2015</t>
+  </si>
+  <si>
+    <t>Eurostat (hlth_silc_02)</t>
+  </si>
+  <si>
+    <t>http://unstats.un.org/unsd/mdg/SeriesDetail.aspx?srid=764&amp;crid=</t>
+  </si>
+  <si>
+    <t>UN Statistics</t>
+  </si>
+  <si>
+    <t>Accessed 26 May 2015</t>
+  </si>
+  <si>
+    <t>Accessed 25 May 2015</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
       <t xml:space="preserve">Figure 30. </t>
     </r>
     <r>
       <rPr>
         <sz val="11"/>
-        <color theme="1"/>
         <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
@@ -322,221 +629,44 @@
     </r>
   </si>
   <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">Figure 34. </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Differences among women aged 65+ in EU countries for self-rated health very good-good by wealth quintiles, 2013</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">Figure 37. </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Long-term pyschological consequences of violence as a result of physical and sexual violence by a partner reported by women 60+ years in the EU</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">Figure 38. </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Differences among older women by age in poverty risk for 2013</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">Figure 5. </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Global Gender Gap for 47 Member States of the WHO European Region 2014</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">Figure 27c. </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">Unmet needs for family planning, total, percentage (last year available) </t>
-    </r>
-  </si>
-  <si>
-    <t>countries</t>
-  </si>
-  <si>
-    <t>number of years</t>
-  </si>
-  <si>
-    <t>Beyond the mortality advantage</t>
-  </si>
-  <si>
-    <t>as in doc</t>
-  </si>
-  <si>
-    <t>Note</t>
-  </si>
-  <si>
-    <t>sub regions</t>
-  </si>
-  <si>
-    <t>deaths and DALYs</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Score </t>
-  </si>
-  <si>
-    <t>percentage</t>
-  </si>
-  <si>
-    <t>Are we maximazing the education gain?</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">Figure 16a. The </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Risk of poverty and social exclusion for girls age less than 6 years in the EU, 2013</t>
-    </r>
-  </si>
-  <si>
-    <t>prevalence</t>
-  </si>
-  <si>
-    <t>Notes: Justification of wife-beating among adolescents – The percentage of boys and girls aged 15–19 who consider a husband to be justified in hitting or beating his wife for at least one of the specified reasons: if his wife burns the food, argues with him, goes out without telling him, neglects the children or refuses sexual relations. Data on male attitudes not availble for Georgia, Montenegro, Tajikistan, TFYR of Macedonia and Turkey most likely because the question is not asked of males. * Data refer to the most recent year available during the period specified in the column heading</t>
-  </si>
-  <si>
-    <t>Notes: Quintile 1 is the lowest equivalised income (lowest 20%) and Quintile 5 is the highest equivalised income. Data for the Czech Republic, Croatia, Serbia and UK(5th quintile only) is noted as having low reliability.</t>
-  </si>
-  <si>
-    <t>number of responses</t>
-  </si>
-  <si>
-    <t>Notes:</t>
-  </si>
-  <si>
-    <t>X and Y lables are as they should be in the graphs as per current draft. However, you will probably change them if presenting the data in a different form, as with the example you shown as on violence Fig 37.</t>
-  </si>
-  <si>
-    <t>Number and name of figure as per draft document</t>
-  </si>
-  <si>
-    <t>Proposed subtitle</t>
-  </si>
-  <si>
-    <t>Page no (in draft doc)</t>
-  </si>
-  <si>
-    <t>Reference no (as per in draft doc)</t>
-  </si>
-  <si>
-    <t>Fig. 15: we have not found an explanation in the data for X lable. Sarah is looking into it.</t>
-  </si>
-  <si>
-    <t>Source was wrong. It is the 2014 Unicef report</t>
-  </si>
-  <si>
-    <t>Girls opportunities for early development</t>
-  </si>
-  <si>
-    <t>Unequal pay for women in all countries</t>
+    <t>Will wait to change until you have tried the new version</t>
+  </si>
+  <si>
+    <t>European Union Agency for Fundamental Rights (FRA)</t>
+  </si>
+  <si>
+    <t>http://fra.europa.eu/en/vaw-survey-results</t>
+  </si>
+  <si>
+    <t>Accessed 09 July 2015</t>
+  </si>
+  <si>
+    <t>I have inserted the date you accessed the web</t>
+  </si>
+  <si>
+    <t>This source has changed. In the Draft Report it was UNDP data</t>
+  </si>
+  <si>
+    <t>http://ec.europa.eu/eurostat/web/products-datasets/-/hlth_silc_10</t>
+  </si>
+  <si>
+    <t>Problems with the original link. I have changed it</t>
+  </si>
+  <si>
+    <t>No access date in the original excel or draft document. Today's date</t>
+  </si>
+  <si>
+    <t>The gradient of gender inequality in Europe</t>
+  </si>
+  <si>
+    <t>http://hdr.undp.org/en/content/labour-force-participation-rate-female-male-ratio</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -573,8 +703,29 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Cambria"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -584,6 +735,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -597,12 +754,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -615,13 +772,35 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="3" fontId="4" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="3" fontId="6" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -921,450 +1100,667 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H31"/>
+  <dimension ref="A1:M31"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="B25" sqref="B25"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="I19" sqref="I19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.28515625" style="5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="104.140625" style="3" customWidth="1"/>
-    <col min="3" max="3" width="12.85546875" style="3" customWidth="1"/>
+    <col min="1" max="1" width="9.28515625" style="4" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="104.140625" style="2" customWidth="1"/>
+    <col min="3" max="3" width="12.85546875" style="2" customWidth="1"/>
     <col min="4" max="4" width="48.5703125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="22.28515625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="18.85546875" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="12" customWidth="1"/>
+    <col min="8" max="8" width="24.7109375" customWidth="1"/>
+    <col min="9" max="9" width="25.85546875" customWidth="1"/>
+    <col min="10" max="10" width="12" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="34.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:13" ht="42" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="D1" s="16" t="s">
+        <v>35</v>
+      </c>
+      <c r="E1" s="16" t="s">
+        <v>1</v>
+      </c>
+      <c r="F1" s="16" t="s">
+        <v>2</v>
+      </c>
+      <c r="G1" s="17" t="s">
         <v>37</v>
       </c>
-      <c r="C1" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="E1" s="1" t="s">
+      <c r="H1" s="17" t="s">
+        <v>40</v>
+      </c>
+      <c r="I1" s="17" t="s">
+        <v>41</v>
+      </c>
+      <c r="J1" s="17" t="s">
+        <v>42</v>
+      </c>
+      <c r="K1" s="18"/>
+      <c r="L1" s="18"/>
+      <c r="M1" s="16" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+      <c r="A2" s="4">
         <v>1</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="B2" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" s="2">
+        <v>10</v>
+      </c>
+      <c r="D2" t="s">
+        <v>21</v>
+      </c>
+      <c r="E2" t="s">
+        <v>19</v>
+      </c>
+      <c r="F2" t="s">
+        <v>20</v>
+      </c>
+      <c r="G2" s="4">
+        <v>34</v>
+      </c>
+      <c r="H2" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="I2" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="J2" s="7" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A3" s="4">
         <v>2</v>
       </c>
-      <c r="G1" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" s="5">
-        <v>1</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="C2" s="3">
-        <v>10</v>
-      </c>
-      <c r="D2" t="s">
+      <c r="B3" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" s="2">
+        <v>11</v>
+      </c>
+      <c r="E3" t="s">
         <v>22</v>
       </c>
-      <c r="E2" t="s">
-        <v>20</v>
-      </c>
-      <c r="F2" t="s">
-        <v>21</v>
-      </c>
-      <c r="G2" s="5">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" s="5">
-        <v>2</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="C3" s="3">
-        <v>11</v>
-      </c>
-      <c r="E3" t="s">
-        <v>23</v>
-      </c>
       <c r="F3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="G3">
         <v>39</v>
       </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" s="5">
+      <c r="H3" t="s">
+        <v>55</v>
+      </c>
+      <c r="I3" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="J3" t="s">
+        <v>65</v>
+      </c>
+      <c r="M3" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A4" s="4">
         <v>3</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="B4" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="3">
+      <c r="C4" s="2">
         <v>13</v>
       </c>
       <c r="E4" t="s">
+        <v>24</v>
+      </c>
+      <c r="F4" t="s">
         <v>25</v>
-      </c>
-      <c r="F4" t="s">
-        <v>26</v>
       </c>
       <c r="G4">
         <v>41</v>
       </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" s="5">
+      <c r="H4" t="s">
+        <v>47</v>
+      </c>
+      <c r="I4" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="J4" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A5" s="4">
         <v>4</v>
       </c>
-      <c r="B5" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="C5" s="3">
+      <c r="B5" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C5" s="2">
         <v>15</v>
       </c>
+      <c r="D5" t="s">
+        <v>87</v>
+      </c>
       <c r="E5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="G5">
         <v>44</v>
       </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" s="5">
+      <c r="H5" t="s">
+        <v>51</v>
+      </c>
+      <c r="I5" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="J5" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A6" s="4">
         <v>5</v>
       </c>
-      <c r="B6" s="3" t="s">
+      <c r="B6" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C6" s="3">
+      <c r="C6" s="2">
         <v>21</v>
       </c>
       <c r="D6" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F6" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="G6">
         <v>62</v>
       </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7" s="5">
+      <c r="H6" t="s">
+        <v>45</v>
+      </c>
+      <c r="I6" s="6" t="s">
+        <v>88</v>
+      </c>
+      <c r="J6" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A7" s="4">
         <v>6</v>
       </c>
-      <c r="B7" s="3" t="s">
+      <c r="B7" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C7" s="3">
+      <c r="C7" s="2">
         <v>24</v>
       </c>
       <c r="D7" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="E7" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F7" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="G7">
         <v>72</v>
       </c>
-    </row>
-    <row r="8" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A8" s="5">
+      <c r="H7" t="s">
+        <v>53</v>
+      </c>
+      <c r="I7" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="J7" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+      <c r="A8" s="4">
         <v>7</v>
       </c>
-      <c r="B8" s="3" t="s">
+      <c r="B8" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C8" s="3">
+      <c r="C8" s="2">
         <v>32</v>
       </c>
       <c r="E8" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F8" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="G8">
         <v>108</v>
       </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9" s="5">
+      <c r="H8" t="s">
+        <v>55</v>
+      </c>
+      <c r="I8" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="J8" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A9" s="4">
         <v>8</v>
       </c>
-      <c r="B9" s="6" t="s">
+      <c r="B9" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="C9" s="6">
+      <c r="C9" s="9">
         <v>39</v>
       </c>
-      <c r="D9" s="7" t="s">
-        <v>43</v>
-      </c>
-      <c r="E9" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="F9" s="7"/>
-      <c r="G9" s="7">
+      <c r="D9" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="E9" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="F9" s="10"/>
+      <c r="G9" s="10">
         <v>121</v>
       </c>
-      <c r="H9" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A10" s="5">
+      <c r="H9" s="10" t="s">
+        <v>58</v>
+      </c>
+      <c r="I9" s="11" t="s">
+        <v>59</v>
+      </c>
+      <c r="J9" s="10" t="s">
+        <v>60</v>
+      </c>
+      <c r="M9" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A10" s="4">
         <v>9</v>
       </c>
-      <c r="B10" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="C10" s="3">
+      <c r="B10" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C10" s="2">
         <v>41</v>
       </c>
       <c r="E10" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F10" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="G10">
         <v>80</v>
       </c>
-    </row>
-    <row r="11" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A11" s="5">
+      <c r="H10" t="s">
+        <v>53</v>
+      </c>
+      <c r="I10" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="J10" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+      <c r="A11" s="4">
         <v>10</v>
       </c>
-      <c r="B11" s="3" t="s">
+      <c r="B11" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="C11" s="3">
+      <c r="C11" s="2">
         <v>50</v>
       </c>
       <c r="E11" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F11" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="G11">
         <v>186</v>
       </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A12" s="5">
+      <c r="H11" t="s">
+        <v>64</v>
+      </c>
+      <c r="I11" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="J11" s="5" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A12" s="4">
         <v>11</v>
       </c>
-      <c r="B12" s="3" t="s">
+      <c r="B12" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="C12" s="3">
+      <c r="C12" s="2">
         <v>56</v>
       </c>
       <c r="E12" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F12" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="G12">
         <v>203</v>
       </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A13" s="5">
+      <c r="H12" t="s">
+        <v>45</v>
+      </c>
+      <c r="I12" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="J12" t="s">
+        <v>68</v>
+      </c>
+      <c r="M12" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A13" s="4">
         <v>12</v>
       </c>
-      <c r="B13" s="3" t="s">
+      <c r="B13" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="C13" s="3">
+      <c r="C13" s="2">
         <v>57</v>
       </c>
       <c r="E13" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F13" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="G13">
         <v>121</v>
       </c>
       <c r="H13" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A14" s="5">
+        <v>58</v>
+      </c>
+      <c r="I13" s="6" t="s">
+        <v>70</v>
+      </c>
+      <c r="J13" t="s">
+        <v>69</v>
+      </c>
+      <c r="M13" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+      <c r="A14" s="4">
         <v>13</v>
       </c>
-      <c r="B14" s="3" t="s">
+      <c r="B14" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="C14" s="3">
+      <c r="C14" s="2">
         <v>63</v>
       </c>
       <c r="E14" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F14" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="G14">
         <v>235</v>
       </c>
       <c r="H14" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A15" s="5">
+        <v>72</v>
+      </c>
+      <c r="I14" s="6" t="s">
+        <v>84</v>
+      </c>
+      <c r="J14" s="8" t="s">
+        <v>76</v>
+      </c>
+      <c r="M14" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A15" s="4">
         <v>14</v>
       </c>
-      <c r="B15" s="3" t="s">
+      <c r="B15" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C15" s="2">
+        <v>73</v>
+      </c>
+      <c r="E15" t="s">
         <v>19</v>
       </c>
-      <c r="C15" s="3">
-        <v>73</v>
-      </c>
-      <c r="E15" t="s">
-        <v>20</v>
-      </c>
       <c r="F15" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="G15">
         <v>278</v>
       </c>
-    </row>
-    <row r="16" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A16" s="5">
+      <c r="H15" t="s">
+        <v>74</v>
+      </c>
+      <c r="I15" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="J15" s="5" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+      <c r="A16" s="4">
         <v>15</v>
       </c>
-      <c r="B16" s="3" t="s">
+      <c r="B16" s="12" t="s">
+        <v>77</v>
+      </c>
+      <c r="C16" s="12">
+        <v>78</v>
+      </c>
+      <c r="D16" s="13"/>
+      <c r="E16" s="13" t="s">
+        <v>22</v>
+      </c>
+      <c r="F16" s="13" t="s">
+        <v>22</v>
+      </c>
+      <c r="G16" s="14">
+        <v>39203</v>
+      </c>
+      <c r="H16" s="14" t="s">
+        <v>45</v>
+      </c>
+      <c r="I16" s="15" t="s">
+        <v>46</v>
+      </c>
+      <c r="J16" s="14" t="s">
+        <v>49</v>
+      </c>
+      <c r="K16" s="13"/>
+      <c r="M16" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+      <c r="A17" s="4">
+        <v>16</v>
+      </c>
+      <c r="B17" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="C16" s="3">
-        <v>78</v>
-      </c>
-      <c r="E16" t="s">
-        <v>23</v>
-      </c>
-      <c r="F16" t="s">
-        <v>23</v>
-      </c>
-      <c r="G16" s="8">
-        <v>39203</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A17" s="5">
-        <v>16</v>
-      </c>
-      <c r="B17" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="C17" s="3">
+      <c r="C17" s="2">
         <v>89</v>
       </c>
       <c r="E17" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F17" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="G17">
         <v>235</v>
       </c>
-    </row>
-    <row r="18" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A18" s="5">
+      <c r="H17" t="s">
+        <v>72</v>
+      </c>
+      <c r="I17" s="6" t="s">
+        <v>84</v>
+      </c>
+      <c r="J17" s="8" t="s">
+        <v>76</v>
+      </c>
+      <c r="M17" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+      <c r="A18" s="4">
         <v>17</v>
       </c>
-      <c r="B18" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="C18" s="3">
+      <c r="B18" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C18" s="2">
         <v>93</v>
       </c>
       <c r="E18" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="F18" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="G18">
         <v>296</v>
       </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A19" s="5">
+      <c r="H18" t="s">
+        <v>79</v>
+      </c>
+      <c r="I18" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="J18" t="s">
+        <v>81</v>
+      </c>
+      <c r="M18" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A19" s="4">
         <v>18</v>
       </c>
-      <c r="B19" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="C19" s="3">
+      <c r="B19" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C19" s="2">
         <v>97</v>
       </c>
       <c r="E19" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F19" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="G19">
         <v>80</v>
       </c>
-    </row>
-    <row r="22" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B22" s="2" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="B23" s="3" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B25" s="3" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B31" s="4"/>
-      <c r="C31" s="4"/>
+      <c r="H19" t="s">
+        <v>53</v>
+      </c>
+      <c r="I19" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="J19" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="B22" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+      <c r="B23" s="2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="D25" s="6"/>
+    </row>
+    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="D27" s="6"/>
+    </row>
+    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B31" s="3"/>
+      <c r="C31" s="3"/>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="I2" r:id="rId1"/>
+    <hyperlink ref="I3" r:id="rId2"/>
+    <hyperlink ref="I4" r:id="rId3"/>
+    <hyperlink ref="I5" r:id="rId4"/>
+    <hyperlink ref="I6" r:id="rId5"/>
+    <hyperlink ref="I7" r:id="rId6"/>
+    <hyperlink ref="I8" r:id="rId7"/>
+    <hyperlink ref="I9" r:id="rId8"/>
+    <hyperlink ref="I10" r:id="rId9"/>
+    <hyperlink ref="I11" r:id="rId10"/>
+    <hyperlink ref="I12" r:id="rId11"/>
+    <hyperlink ref="I13" r:id="rId12"/>
+    <hyperlink ref="I14" r:id="rId13"/>
+    <hyperlink ref="I15" r:id="rId14"/>
+    <hyperlink ref="I16" r:id="rId15"/>
+    <hyperlink ref="I18" r:id="rId16"/>
+    <hyperlink ref="I19" r:id="rId17"/>
+    <hyperlink ref="I17" r:id="rId18"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="landscape" r:id="rId19"/>
 </worksheet>
 </file>
 

</xml_diff>